<commit_message>
More tests on IRON
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
+++ b/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
@@ -740,7 +740,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>111.3217836438596</v>
+        <v>112.84340945255747</v>
       </c>
     </row>
     <row r="4">
@@ -751,7 +751,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>52469.16847303212</v>
+        <v>52263.1431262652</v>
       </c>
     </row>
     <row r="5">
@@ -762,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>49929.83435027857</v>
+        <v>49919.610559671804</v>
       </c>
     </row>
     <row r="6">
@@ -773,7 +773,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>2673.1684730321313</v>
+        <v>2467.1431262652072</v>
       </c>
     </row>
     <row r="7">
@@ -784,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>2539.510049380525</v>
+        <v>2343.7859699519468</v>
       </c>
     </row>
     <row r="8">
@@ -831,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5343075876139025</v>
+        <v>0.5308083423660894</v>
       </c>
     </row>
     <row r="13">
@@ -842,7 +842,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>97.6809609675536</v>
+        <v>96.57603827332888</v>
       </c>
     </row>
     <row r="14">
@@ -853,7 +853,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>141.70577064630237</v>
+        <v>142.887868983031</v>
       </c>
     </row>
     <row r="15">
@@ -864,7 +864,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>95.44884708572303</v>
+        <v>95.44884708572306</v>
       </c>
     </row>
     <row r="16">
@@ -875,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>22.09108979931446</v>
+        <v>22.017503337030206</v>
       </c>
     </row>
     <row r="17">
@@ -886,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>99.99999999999994</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="18">
@@ -897,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>38.39482262187994</v>
+        <v>38.39482262187991</v>
       </c>
     </row>
     <row r="19">
@@ -930,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5574276500924213</v>
+        <v>0.5573494361384519</v>
       </c>
     </row>
     <row r="22">
@@ -946,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>0.404573804951899</v>
+        <v>0.4023727896790188</v>
       </c>
     </row>
     <row r="24">
@@ -957,7 +957,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="n">
-        <v>16.58268925796842</v>
+        <v>16.40161372463008</v>
       </c>
     </row>
     <row r="25">
@@ -968,7 +968,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>17.534639693169538</v>
+        <v>18.64913214034498</v>
       </c>
     </row>
     <row r="26">
@@ -990,7 +990,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>4.491605370931133</v>
+        <v>4.476945800608419</v>
       </c>
     </row>
     <row r="28">
@@ -1001,7 +1001,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>12.990364158819158</v>
+        <v>13.595467385791132</v>
       </c>
     </row>
     <row r="29">
@@ -1045,7 +1045,7 @@
         <v>6</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3512446913528251</v>
+        <v>0.3512109448371987</v>
       </c>
     </row>
     <row r="33">
@@ -1061,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>37.5384152867733</v>
+        <v>37.33126781772375</v>
       </c>
     </row>
     <row r="35">
@@ -1072,7 +1072,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="n">
-        <v>797.0916524655247</v>
+        <v>788.8369109468399</v>
       </c>
     </row>
     <row r="36">
@@ -1083,7 +1083,7 @@
         <v>8</v>
       </c>
       <c r="C36" t="n">
-        <v>616.6599238333979</v>
+        <v>537.6088759926045</v>
       </c>
     </row>
     <row r="37">
@@ -1094,7 +1094,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>1.5514929728291236</v>
+        <v>1.5680932681558488</v>
       </c>
     </row>
     <row r="38">
@@ -1105,7 +1105,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="n">
-        <v>270.88704679019213</v>
+        <v>270.00861556829545</v>
       </c>
     </row>
     <row r="39">
@@ -1116,7 +1116,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="n">
-        <v>671.6959858942153</v>
+        <v>564.3780993874409</v>
       </c>
     </row>
     <row r="40">
@@ -1127,7 +1127,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>21.57065020054756</v>
+        <v>21.583618213096315</v>
       </c>
     </row>
     <row r="41">
@@ -1138,7 +1138,7 @@
         <v>8</v>
       </c>
       <c r="C41" t="n">
-        <v>122.54649450899547</v>
+        <v>122.50075931938022</v>
       </c>
     </row>
     <row r="42">
@@ -1149,7 +1149,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.031612571950745405</v>
+        <v>-0.03027056158975938</v>
       </c>
     </row>
     <row r="43">
@@ -1176,7 +1176,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="n">
-        <v>52431.80598437237</v>
+        <v>52226.065261806056</v>
       </c>
     </row>
     <row r="46">
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="n">
-        <v>51634.71433190684</v>
+        <v>51437.228350859215</v>
       </c>
     </row>
     <row r="47">
@@ -1198,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="n">
-        <v>51018.05440807344</v>
+        <v>50899.6194748666</v>
       </c>
     </row>
     <row r="48">
@@ -1209,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="n">
-        <v>51016.5029151006</v>
+        <v>50898.051381598445</v>
       </c>
     </row>
     <row r="49">
@@ -1220,7 +1220,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="n">
-        <v>50745.61586831041</v>
+        <v>50628.04276603015</v>
       </c>
     </row>
     <row r="50">
@@ -1231,7 +1231,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="n">
-        <v>50073.91988241619</v>
+        <v>50063.664666642704</v>
       </c>
     </row>
     <row r="51">
@@ -1242,7 +1242,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="n">
-        <v>50052.34923221564</v>
+        <v>50042.08104842961</v>
       </c>
     </row>
     <row r="52">
@@ -1253,7 +1253,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="n">
-        <v>49929.80273770663</v>
+        <v>49919.58028911022</v>
       </c>
     </row>
     <row r="53">
@@ -1264,7 +1264,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="n">
-        <v>49929.83435027858</v>
+        <v>49919.61055967181</v>
       </c>
     </row>
     <row r="54">
@@ -1275,7 +1275,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="n">
-        <v>49929.83435027857</v>
+        <v>49919.610559671804</v>
       </c>
     </row>
     <row r="55">
@@ -1307,7 +1307,7 @@
         <v>59</v>
       </c>
       <c r="C58" t="n">
-        <v>147.2287526559152</v>
+        <v>147.06581114238537</v>
       </c>
     </row>
     <row r="59">
@@ -1329,7 +1329,7 @@
         <v>17</v>
       </c>
       <c r="C60" t="n">
-        <v>0.22260203694624983</v>
+        <v>0.2223556780512614</v>
       </c>
     </row>
     <row r="61">
@@ -1351,7 +1351,7 @@
         <v>17</v>
       </c>
       <c r="C62" t="n">
-        <v>2.126189561697079</v>
+        <v>2.126695251478622</v>
       </c>
     </row>
     <row r="63">
@@ -1373,7 +1373,7 @@
         <v>17</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0926496353807621</v>
+        <v>0.09267083118915845</v>
       </c>
     </row>
     <row r="65">
@@ -1395,7 +1395,7 @@
         <v>17</v>
       </c>
       <c r="C66" t="n">
-        <v>22.948709435920396</v>
+        <v>22.94891741218594</v>
       </c>
     </row>
     <row r="67">
@@ -1406,7 +1406,7 @@
         <v>70</v>
       </c>
       <c r="C67" t="n">
-        <v>46611.949108155946</v>
+        <v>46611.9489095388</v>
       </c>
     </row>
     <row r="68">
@@ -1417,7 +1417,7 @@
         <v>70</v>
       </c>
       <c r="C68" t="n">
-        <v>37395.09870081817</v>
+        <v>37403.91950088453</v>
       </c>
     </row>
     <row r="69">
@@ -1439,7 +1439,7 @@
         <v>70</v>
       </c>
       <c r="C70" t="n">
-        <v>7036.575356478633</v>
+        <v>7022.615112008484</v>
       </c>
     </row>
     <row r="71">
@@ -1504,7 +1504,7 @@
         <v>17</v>
       </c>
       <c r="C77" t="n">
-        <v>0.4154682889938561</v>
+        <v>0.41383800477273924</v>
       </c>
     </row>
     <row r="78">
@@ -1515,7 +1515,7 @@
         <v>17</v>
       </c>
       <c r="C78" t="n">
-        <v>1.091867864657074</v>
+        <v>1.0876918253545205</v>
       </c>
     </row>
     <row r="79">
@@ -1526,7 +1526,7 @@
         <v>17</v>
       </c>
       <c r="C79" t="n">
-        <v>0.029624798604174715</v>
+        <v>0.029563764164287156</v>
       </c>
     </row>
     <row r="80">
@@ -1537,7 +1537,7 @@
         <v>17</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0737133924294191</v>
+        <v>0.07332278232273193</v>
       </c>
     </row>
     <row r="81">
@@ -1548,7 +1548,7 @@
         <v>17</v>
       </c>
       <c r="C81" t="n">
-        <v>14.024341381862035</v>
+        <v>13.9981499809369</v>
       </c>
     </row>
     <row r="82">
@@ -1559,7 +1559,7 @@
         <v>17</v>
       </c>
       <c r="C82" t="n">
-        <v>14.812340453636596</v>
+        <v>14.83429557496904</v>
       </c>
     </row>
     <row r="83">
@@ -1570,7 +1570,7 @@
         <v>70</v>
       </c>
       <c r="C83" t="n">
-        <v>24089.471436028558</v>
+        <v>24073.62015582046</v>
       </c>
     </row>
     <row r="84">
@@ -1581,7 +1581,7 @@
         <v>70</v>
       </c>
       <c r="C84" t="n">
-        <v>11058.292826177614</v>
+        <v>11059.118118010332</v>
       </c>
     </row>
     <row r="85">
@@ -1592,7 +1592,7 @@
         <v>70</v>
       </c>
       <c r="C85" t="n">
-        <v>8242.460890642398</v>
+        <v>8221.467394931173</v>
       </c>
     </row>
     <row r="86">
@@ -1603,7 +1603,7 @@
         <v>70</v>
       </c>
       <c r="C86" t="n">
-        <v>7850.13349417967</v>
+        <v>7807.31702248335</v>
       </c>
     </row>
     <row r="87">
@@ -1624,7 +1624,7 @@
         <v>59</v>
       </c>
       <c r="C89" t="n">
-        <v>484.28579957027137</v>
+        <v>459.08300177402543</v>
       </c>
     </row>
     <row r="90">
@@ -1635,7 +1635,7 @@
         <v>59</v>
       </c>
       <c r="C90" t="n">
-        <v>485.66476888215806</v>
+        <v>460.52731432613206</v>
       </c>
     </row>
     <row r="91">
@@ -1646,7 +1646,7 @@
         <v>17</v>
       </c>
       <c r="C91" t="n">
-        <v>0.8216140748357936</v>
+        <v>0.7788563201937818</v>
       </c>
     </row>
     <row r="92">
@@ -1657,7 +1657,7 @@
         <v>17</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8239535623789305</v>
+        <v>0.7813066656763994</v>
       </c>
     </row>
     <row r="93">
@@ -1668,7 +1668,7 @@
         <v>17</v>
       </c>
       <c r="C93" t="n">
-        <v>0.31471200573089897</v>
+        <v>0.348875229484687</v>
       </c>
     </row>
     <row r="94">
@@ -1679,7 +1679,7 @@
         <v>17</v>
       </c>
       <c r="C94" t="n">
-        <v>0.307316933319692</v>
+        <v>0.34125228922845885</v>
       </c>
     </row>
     <row r="95">
@@ -1690,7 +1690,7 @@
         <v>17</v>
       </c>
       <c r="C95" t="n">
-        <v>0.024749736221345076</v>
+        <v>0.025547831227245296</v>
       </c>
     </row>
     <row r="96">
@@ -1701,7 +1701,7 @@
         <v>17</v>
       </c>
       <c r="C96" t="n">
-        <v>0.024576978216942744</v>
+        <v>0.025369749949183916</v>
       </c>
     </row>
     <row r="97">
@@ -1712,7 +1712,7 @@
         <v>17</v>
       </c>
       <c r="C97" t="n">
-        <v>12.71577211637027</v>
+        <v>13.655766956556047</v>
       </c>
     </row>
     <row r="98">
@@ -1723,7 +1723,7 @@
         <v>17</v>
       </c>
       <c r="C98" t="n">
-        <v>12.504260312516188</v>
+        <v>13.45114910127193</v>
       </c>
     </row>
     <row r="99">
@@ -1734,7 +1734,7 @@
         <v>70</v>
       </c>
       <c r="C99" t="n">
-        <v>8952.272677352392</v>
+        <v>8304.160256122626</v>
       </c>
     </row>
     <row r="100">
@@ -1745,7 +1745,7 @@
         <v>70</v>
       </c>
       <c r="C100" t="n">
-        <v>8940.482191946496</v>
+        <v>8298.244601761078</v>
       </c>
     </row>
     <row r="101">
@@ -1756,7 +1756,7 @@
         <v>70</v>
       </c>
       <c r="C101" t="n">
-        <v>8952.272677352392</v>
+        <v>8304.160256122626</v>
       </c>
     </row>
     <row r="102">
@@ -1767,7 +1767,7 @@
         <v>70</v>
       </c>
       <c r="C102" t="n">
-        <v>8940.482191946496</v>
+        <v>8298.244601761078</v>
       </c>
     </row>
     <row r="103">
@@ -1832,7 +1832,7 @@
         <v>17</v>
       </c>
       <c r="C109" t="n">
-        <v>0.5641559818275375</v>
+        <v>0.5628463321985737</v>
       </c>
     </row>
     <row r="110">
@@ -1843,7 +1843,7 @@
         <v>17</v>
       </c>
       <c r="C110" t="n">
-        <v>0.5638119644814734</v>
+        <v>0.5625034934743327</v>
       </c>
     </row>
     <row r="111">
@@ -1854,7 +1854,7 @@
         <v>17</v>
       </c>
       <c r="C111" t="n">
-        <v>0.032532257073064265</v>
+        <v>0.03247844996867854</v>
       </c>
     </row>
     <row r="112">
@@ -1865,7 +1865,7 @@
         <v>17</v>
       </c>
       <c r="C112" t="n">
-        <v>0.032518123081162316</v>
+        <v>0.03246436440058862</v>
       </c>
     </row>
     <row r="113">
@@ -1876,7 +1876,7 @@
         <v>17</v>
       </c>
       <c r="C113" t="n">
-        <v>17.341433782491585</v>
+        <v>17.329839716531104</v>
       </c>
     </row>
     <row r="114">
@@ -1887,7 +1887,7 @@
         <v>17</v>
       </c>
       <c r="C114" t="n">
-        <v>17.338391981426767</v>
+        <v>17.326798286681804</v>
       </c>
     </row>
     <row r="115">
@@ -1898,7 +1898,7 @@
         <v>70</v>
       </c>
       <c r="C115" t="n">
-        <v>-311.0648125400993</v>
+        <v>-311.0648126141039</v>
       </c>
     </row>
     <row r="116">
@@ -1909,7 +1909,7 @@
         <v>70</v>
       </c>
       <c r="C116" t="n">
-        <v>808.723437359591</v>
+        <v>809.9170717580963</v>
       </c>
     </row>
     <row r="117">
@@ -1920,7 +1920,7 @@
         <v>70</v>
       </c>
       <c r="C117" t="n">
-        <v>7132.1423557438675</v>
+        <v>7120.31593457726</v>
       </c>
     </row>
     <row r="118">
@@ -1931,7 +1931,7 @@
         <v>70</v>
       </c>
       <c r="C118" t="n">
-        <v>7129.035804240933</v>
+        <v>7117.22002628589</v>
       </c>
     </row>
     <row r="119">
@@ -1996,7 +1996,7 @@
         <v>17</v>
       </c>
       <c r="C125" t="n">
-        <v>0.40425347679986806</v>
+        <v>0.40331486984889353</v>
       </c>
     </row>
     <row r="126">
@@ -2007,7 +2007,7 @@
         <v>17</v>
       </c>
       <c r="C126" t="n">
-        <v>0.6112437681927804</v>
+        <v>0.6098275704612877</v>
       </c>
     </row>
     <row r="127">
@@ -2018,7 +2018,7 @@
         <v>17</v>
       </c>
       <c r="C127" t="n">
-        <v>0.02920493943370731</v>
+        <v>0.029169799947729794</v>
       </c>
     </row>
     <row r="128">
@@ -2029,7 +2029,7 @@
         <v>17</v>
       </c>
       <c r="C128" t="n">
-        <v>0.03821842225421682</v>
+        <v>0.03814301431355167</v>
       </c>
     </row>
     <row r="129">
@@ -2040,7 +2040,7 @@
         <v>17</v>
       </c>
       <c r="C129" t="n">
-        <v>13.841955663612607</v>
+        <v>13.826453063497352</v>
       </c>
     </row>
     <row r="130">
@@ -2051,7 +2051,7 @@
         <v>17</v>
       </c>
       <c r="C130" t="n">
-        <v>15.993432803870885</v>
+        <v>15.987922859170169</v>
       </c>
     </row>
     <row r="131">
@@ -2084,7 +2084,7 @@
         <v>70</v>
       </c>
       <c r="C133" t="n">
-        <v>7956.682571278696</v>
+        <v>7946.904670725951</v>
       </c>
     </row>
     <row r="134">
@@ -2095,7 +2095,7 @@
         <v>70</v>
       </c>
       <c r="C134" t="n">
-        <v>6982.0789150678</v>
+        <v>6968.1702634312605</v>
       </c>
     </row>
     <row r="135">
@@ -2116,7 +2116,7 @@
         <v>59</v>
       </c>
       <c r="C137" t="n">
-        <v>461.6611808872903</v>
+        <v>441.21068121021403</v>
       </c>
     </row>
     <row r="138">
@@ -2127,7 +2127,7 @@
         <v>59</v>
       </c>
       <c r="C138" t="n">
-        <v>461.6611808872903</v>
+        <v>441.21068121021403</v>
       </c>
     </row>
     <row r="139">
@@ -2138,7 +2138,7 @@
         <v>17</v>
       </c>
       <c r="C139" t="n">
-        <v>0.7369292919263221</v>
+        <v>0.704285065228287</v>
       </c>
     </row>
     <row r="140">
@@ -2149,7 +2149,7 @@
         <v>17</v>
       </c>
       <c r="C140" t="n">
-        <v>0.7369292919263221</v>
+        <v>0.704285065228287</v>
       </c>
     </row>
     <row r="141">
@@ -2160,7 +2160,7 @@
         <v>17</v>
       </c>
       <c r="C141" t="n">
-        <v>0.2026162542837819</v>
+        <v>0.22132046496662092</v>
       </c>
     </row>
     <row r="142">
@@ -2171,7 +2171,7 @@
         <v>17</v>
       </c>
       <c r="C142" t="n">
-        <v>0.19821489017607719</v>
+        <v>0.217171901093037</v>
       </c>
     </row>
     <row r="143">
@@ -2182,7 +2182,7 @@
         <v>17</v>
       </c>
       <c r="C143" t="n">
-        <v>0.02256092885805613</v>
+        <v>0.022849750062349312</v>
       </c>
     </row>
     <row r="144">
@@ -2193,7 +2193,7 @@
         <v>17</v>
       </c>
       <c r="C144" t="n">
-        <v>0.022497079317791584</v>
+        <v>0.022772084157704518</v>
       </c>
     </row>
     <row r="145">
@@ -2204,7 +2204,7 @@
         <v>17</v>
       </c>
       <c r="C145" t="n">
-        <v>8.98084717870253</v>
+        <v>9.685903100152585</v>
       </c>
     </row>
     <row r="146">
@@ -2215,7 +2215,7 @@
         <v>17</v>
       </c>
       <c r="C146" t="n">
-        <v>8.810694373972401</v>
+        <v>9.536759990392046</v>
       </c>
     </row>
     <row r="147">
@@ -2226,7 +2226,7 @@
         <v>70</v>
       </c>
       <c r="C147" t="n">
-        <v>12457.057833945677</v>
+        <v>11523.52312714743</v>
       </c>
     </row>
     <row r="148">
@@ -2237,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="C148" t="n">
-        <v>12445.464391336833</v>
+        <v>11507.889093627313</v>
       </c>
     </row>
     <row r="149">
@@ -2248,7 +2248,7 @@
         <v>70</v>
       </c>
       <c r="C149" t="n">
-        <v>12457.057833945677</v>
+        <v>11523.52312714743</v>
       </c>
     </row>
     <row r="150">
@@ -2259,7 +2259,7 @@
         <v>70</v>
       </c>
       <c r="C150" t="n">
-        <v>12445.464391336833</v>
+        <v>11507.889093627313</v>
       </c>
     </row>
     <row r="151">
@@ -2324,7 +2324,7 @@
         <v>17</v>
       </c>
       <c r="C157" t="n">
-        <v>0.5533954471594784</v>
+        <v>0.5532821109211329</v>
       </c>
     </row>
     <row r="158">
@@ -2335,7 +2335,7 @@
         <v>17</v>
       </c>
       <c r="C158" t="n">
-        <v>0.5526559730475576</v>
+        <v>0.5525422808074715</v>
       </c>
     </row>
     <row r="159">
@@ -2346,7 +2346,7 @@
         <v>17</v>
       </c>
       <c r="C159" t="n">
-        <v>0.03209772622566322</v>
+        <v>0.03209357219044354</v>
       </c>
     </row>
     <row r="160">
@@ -2357,7 +2357,7 @@
         <v>17</v>
       </c>
       <c r="C160" t="n">
-        <v>0.03207062278946487</v>
+        <v>0.03206645570595816</v>
       </c>
     </row>
     <row r="161">
@@ -2368,7 +2368,7 @@
         <v>17</v>
       </c>
       <c r="C161" t="n">
-        <v>17.240954803739964</v>
+        <v>17.23965495763301</v>
       </c>
     </row>
     <row r="162">
@@ -2379,7 +2379,7 @@
         <v>17</v>
       </c>
       <c r="C162" t="n">
-        <v>17.232467753295516</v>
+        <v>17.231161618675724</v>
       </c>
     </row>
     <row r="163">
@@ -2390,7 +2390,7 @@
         <v>70</v>
       </c>
       <c r="C163" t="n">
-        <v>1130.1946133552606</v>
+        <v>1131.8962165037506</v>
       </c>
     </row>
     <row r="164">
@@ -2401,7 +2401,7 @@
         <v>70</v>
       </c>
       <c r="C164" t="n">
-        <v>445.6387321062796</v>
+        <v>445.58197273788926</v>
       </c>
     </row>
     <row r="165">
@@ -2412,7 +2412,7 @@
         <v>70</v>
       </c>
       <c r="C165" t="n">
-        <v>7034.972385892438</v>
+        <v>7033.948934994985</v>
       </c>
     </row>
     <row r="166">
@@ -2423,7 +2423,7 @@
         <v>70</v>
       </c>
       <c r="C166" t="n">
-        <v>7028.294773731165</v>
+        <v>7027.268108060516</v>
       </c>
     </row>
     <row r="167">
@@ -2488,7 +2488,7 @@
         <v>17</v>
       </c>
       <c r="C173" t="n">
-        <v>0.7189555552356247</v>
+        <v>0.7188080623029574</v>
       </c>
     </row>
     <row r="174">
@@ -2499,7 +2499,7 @@
         <v>17</v>
       </c>
       <c r="C174" t="n">
-        <v>0.7176346188878386</v>
+        <v>0.717487619075011</v>
       </c>
     </row>
     <row r="175">
@@ -2510,7 +2510,7 @@
         <v>17</v>
       </c>
       <c r="C175" t="n">
-        <v>0.03944756059120251</v>
+        <v>0.0394401926933973</v>
       </c>
     </row>
     <row r="176">
@@ -2521,7 +2521,7 @@
         <v>17</v>
       </c>
       <c r="C176" t="n">
-        <v>0.03938157421584426</v>
+        <v>0.03937423095146737</v>
       </c>
     </row>
     <row r="177">
@@ -2532,7 +2532,7 @@
         <v>17</v>
       </c>
       <c r="C177" t="n">
-        <v>18.225602406349157</v>
+        <v>18.22526750543218</v>
       </c>
     </row>
     <row r="178">
@@ -2543,7 +2543,7 @@
         <v>17</v>
       </c>
       <c r="C178" t="n">
-        <v>18.222598592798633</v>
+        <v>18.22226369219466</v>
       </c>
     </row>
     <row r="179">
@@ -2554,7 +2554,7 @@
         <v>70</v>
       </c>
       <c r="C179" t="n">
-        <v>6054.479788035808</v>
+        <v>6053.34895034462</v>
       </c>
     </row>
     <row r="180">
@@ -2565,7 +2565,7 @@
         <v>70</v>
       </c>
       <c r="C180" t="n">
-        <v>6044.3520850827035</v>
+        <v>6043.225028172676</v>
       </c>
     </row>
     <row r="181">
@@ -2576,7 +2576,7 @@
         <v>70</v>
       </c>
       <c r="C181" t="n">
-        <v>6054.479788035808</v>
+        <v>6053.34895034462</v>
       </c>
     </row>
     <row r="182">
@@ -2587,7 +2587,7 @@
         <v>70</v>
       </c>
       <c r="C182" t="n">
-        <v>6044.3520850827035</v>
+        <v>6043.225028172676</v>
       </c>
     </row>
     <row r="183">
@@ -2652,7 +2652,7 @@
         <v>17</v>
       </c>
       <c r="C189" t="n">
-        <v>0.5513919548920491</v>
+        <v>0.5512790648823496</v>
       </c>
     </row>
     <row r="190">
@@ -2663,7 +2663,7 @@
         <v>17</v>
       </c>
       <c r="C190" t="n">
-        <v>0.5513542365450854</v>
+        <v>0.5512413716588563</v>
       </c>
     </row>
     <row r="191">
@@ -2674,7 +2674,7 @@
         <v>17</v>
       </c>
       <c r="C191" t="n">
-        <v>0.032024293601087474</v>
+        <v>0.03202015592117955</v>
       </c>
     </row>
     <row r="192">
@@ -2685,7 +2685,7 @@
         <v>17</v>
       </c>
       <c r="C192" t="n">
-        <v>0.032022911136449485</v>
+        <v>0.03201877437737485</v>
       </c>
     </row>
     <row r="193">
@@ -2696,7 +2696,7 @@
         <v>17</v>
       </c>
       <c r="C193" t="n">
-        <v>17.217927169932175</v>
+        <v>17.21662649736534</v>
       </c>
     </row>
     <row r="194">
@@ -2707,7 +2707,7 @@
         <v>17</v>
       </c>
       <c r="C194" t="n">
-        <v>17.21749263193991</v>
+        <v>17.216192136585192</v>
       </c>
     </row>
     <row r="195">
@@ -2718,7 +2718,7 @@
         <v>70</v>
       </c>
       <c r="C195" t="n">
-        <v>-54.63182206511402</v>
+        <v>-58.59660992986095</v>
       </c>
     </row>
     <row r="196">
@@ -2729,7 +2729,7 @@
         <v>70</v>
       </c>
       <c r="C196" t="n">
-        <v>13.13648857717249</v>
+        <v>13.594577309080737</v>
       </c>
     </row>
     <row r="197">
@@ -2740,7 +2740,7 @@
         <v>70</v>
       </c>
       <c r="C197" t="n">
-        <v>7016.880414700567</v>
+        <v>7015.860993344899</v>
       </c>
     </row>
     <row r="198">
@@ -2751,7 +2751,7 @@
         <v>70</v>
       </c>
       <c r="C198" t="n">
-        <v>7016.539809818896</v>
+        <v>7015.520615333634</v>
       </c>
     </row>
     <row r="199">
@@ -2772,7 +2772,7 @@
         <v>59</v>
       </c>
       <c r="C201" t="n">
-        <v>117.31576827160768</v>
+        <v>117.3037566830413</v>
       </c>
     </row>
     <row r="202">
@@ -2794,7 +2794,7 @@
         <v>17</v>
       </c>
       <c r="C203" t="n">
-        <v>0.17738434640210213</v>
+        <v>0.17736618458277903</v>
       </c>
     </row>
     <row r="204">
@@ -2904,7 +2904,7 @@
         <v>70</v>
       </c>
       <c r="C213" t="n">
-        <v>4559.668792783809</v>
+        <v>4558.735009648629</v>
       </c>
     </row>
     <row r="214">

</xml_diff>

<commit_message>
More work on ACPerformanceManager: mission profile analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
+++ b/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="328">
   <si>
     <t>Description</t>
   </si>
@@ -23,18 +23,24 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Total mission distance</t>
+    <t>Mission distance</t>
   </si>
   <si>
     <t>nmi</t>
   </si>
   <si>
+    <t>Total mission distance (plus reserves)</t>
+  </si>
+  <si>
+    <t>Block time</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
     <t>Total mission duration</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
     <t>Aircraft mass at mission start</t>
   </si>
   <si>
@@ -47,6 +53,9 @@
     <t>Initial fuel mass for the assigned mission</t>
   </si>
   <si>
+    <t>Block fuel</t>
+  </si>
+  <si>
     <t>Total fuel used</t>
   </si>
   <si>
@@ -98,6 +107,39 @@
     <t>Landing range</t>
   </si>
   <si>
+    <t>Altitude at take-off ending</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>Altitude at climb ending</t>
+  </si>
+  <si>
+    <t>Altitude at cruise ending</t>
+  </si>
+  <si>
+    <t>Altitude at first descent ending</t>
+  </si>
+  <si>
+    <t>Altitude at second climb ending</t>
+  </si>
+  <si>
+    <t>Altitude at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Altitude at second descent ending</t>
+  </si>
+  <si>
+    <t>Altitude at holding ending</t>
+  </si>
+  <si>
+    <t>Altitude at third descent ending</t>
+  </si>
+  <si>
+    <t>Altitude at landing ending</t>
+  </si>
+  <si>
     <t>Take-off duration</t>
   </si>
   <si>
@@ -140,6 +182,9 @@
     <t>First descent used fuel</t>
   </si>
   <si>
+    <t>Second Climb used fuel</t>
+  </si>
+  <si>
     <t>Alternate cruise used fuel</t>
   </si>
   <si>
@@ -197,6 +242,12 @@
     <t>Speed (TAS) at take-off ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at take-off start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at take-off ending</t>
+  </si>
+  <si>
     <t>Mach at take-off start</t>
   </si>
   <si>
@@ -236,6 +287,42 @@
     <t>Drag at take-off ending</t>
   </si>
   <si>
+    <t>Rate of climb at take-off start</t>
+  </si>
+  <si>
+    <t>ft/min</t>
+  </si>
+  <si>
+    <t>Rate of climb at take-off ending</t>
+  </si>
+  <si>
+    <t>Climb angle at take-off start</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>Climb angle at take-off ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at take-off start</t>
+  </si>
+  <si>
+    <t>lb/hr</t>
+  </si>
+  <si>
+    <t>Fuel flow at take-off ending</t>
+  </si>
+  <si>
+    <t>SFC at take-off start</t>
+  </si>
+  <si>
+    <t>lb/(lb*hr)</t>
+  </si>
+  <si>
+    <t>SFC at take-off ending</t>
+  </si>
+  <si>
     <t>CLIMB</t>
   </si>
   <si>
@@ -245,6 +332,12 @@
     <t>Speed (TAS) at climb ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at climb start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at climb ending</t>
+  </si>
+  <si>
     <t>Mach at climb start</t>
   </si>
   <si>
@@ -281,6 +374,30 @@
     <t>Drag at climb ending</t>
   </si>
   <si>
+    <t>Rate of climb at climb start</t>
+  </si>
+  <si>
+    <t>Rate of climb at climb ending</t>
+  </si>
+  <si>
+    <t>Climb angle at climb start</t>
+  </si>
+  <si>
+    <t>Climb angle at climb ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at climb start</t>
+  </si>
+  <si>
+    <t>Fuel flow at climb ending</t>
+  </si>
+  <si>
+    <t>SFC at climb start</t>
+  </si>
+  <si>
+    <t>SFC at climb ending</t>
+  </si>
+  <si>
     <t>CRUISE</t>
   </si>
   <si>
@@ -290,6 +407,12 @@
     <t>Speed (TAS) at cruise ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at cruise start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at cruise ending</t>
+  </si>
+  <si>
     <t>Mach at cruise start</t>
   </si>
   <si>
@@ -326,6 +449,30 @@
     <t>Drag at cruise ending</t>
   </si>
   <si>
+    <t>Rate of climb at cruise start</t>
+  </si>
+  <si>
+    <t>Rate of climb at cruise ending</t>
+  </si>
+  <si>
+    <t>Climb angle at cruise start</t>
+  </si>
+  <si>
+    <t>Climb angle at cruise ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at cruise start</t>
+  </si>
+  <si>
+    <t>Fuel flow at cruise ending</t>
+  </si>
+  <si>
+    <t>SFC at cruise start</t>
+  </si>
+  <si>
+    <t>SFC at cruise ending</t>
+  </si>
+  <si>
     <t>FIRST DESCENT</t>
   </si>
   <si>
@@ -335,6 +482,12 @@
     <t>Speed (TAS) at first descent ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at first descent start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at first descent ending</t>
+  </si>
+  <si>
     <t>Mach at first descent start</t>
   </si>
   <si>
@@ -365,55 +518,109 @@
     <t>Thrust at first descent ending</t>
   </si>
   <si>
+    <t>Drag at first descent start</t>
+  </si>
+  <si>
+    <t>Drag at first descent ending</t>
+  </si>
+  <si>
+    <t>Rate of climb at first descent start</t>
+  </si>
+  <si>
+    <t>Rate of climb at first descent ending</t>
+  </si>
+  <si>
+    <t>Climb angle at first descent start</t>
+  </si>
+  <si>
+    <t>Climb angle at first descent ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at first descent start</t>
+  </si>
+  <si>
+    <t>Fuel flow at first descent ending</t>
+  </si>
+  <si>
+    <t>SFC at first descent start</t>
+  </si>
+  <si>
+    <t>SFC at first descent ending</t>
+  </si>
+  <si>
+    <t>SECOND CLIMB</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second climb start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second climb ending</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at second climb start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at second climb ending</t>
+  </si>
+  <si>
+    <t>Mach at second climb start</t>
+  </si>
+  <si>
+    <t>Mach at second climb ending</t>
+  </si>
+  <si>
+    <t>CL at second climb start</t>
+  </si>
+  <si>
+    <t>CL at second climb ending</t>
+  </si>
+  <si>
+    <t>CD at second climb start</t>
+  </si>
+  <si>
+    <t>CD at second climb ending</t>
+  </si>
+  <si>
+    <t>Efficiency at second climb start</t>
+  </si>
+  <si>
+    <t>Efficiency at second climb ending</t>
+  </si>
+  <si>
+    <t>Thrust at second climb start</t>
+  </si>
+  <si>
+    <t>Thrust at second climb ending</t>
+  </si>
+  <si>
     <t>Drag at second climb start</t>
   </si>
   <si>
     <t>Drag at second climb ending</t>
   </si>
   <si>
-    <t>SECOND CLIMB</t>
-  </si>
-  <si>
-    <t>Speed (TAS) at second climb start</t>
-  </si>
-  <si>
-    <t>Speed (TAS) at second climb ending</t>
-  </si>
-  <si>
-    <t>Mach at second climb start</t>
-  </si>
-  <si>
-    <t>Mach at second climb ending</t>
-  </si>
-  <si>
-    <t>CL at second climb start</t>
-  </si>
-  <si>
-    <t>CL at second climb ending</t>
-  </si>
-  <si>
-    <t>CD at second climb start</t>
-  </si>
-  <si>
-    <t>CD at second climb ending</t>
-  </si>
-  <si>
-    <t>Efficiency at second climb start</t>
-  </si>
-  <si>
-    <t>Efficiency at second climb ending</t>
-  </si>
-  <si>
-    <t>Thrust at second climb start</t>
-  </si>
-  <si>
-    <t>Thrust at second climb ending</t>
-  </si>
-  <si>
-    <t>Drag at first descent start</t>
-  </si>
-  <si>
-    <t>Drag at first descent ending</t>
+    <t>Rate of climb at second climb start</t>
+  </si>
+  <si>
+    <t>Rate of climb at second climb ending</t>
+  </si>
+  <si>
+    <t>Climb angle at second climb start</t>
+  </si>
+  <si>
+    <t>Climb angle at second climb ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at second climb start</t>
+  </si>
+  <si>
+    <t>Fuel flow at second climb ending</t>
+  </si>
+  <si>
+    <t>SFC at second climb start</t>
+  </si>
+  <si>
+    <t>SFC at second climb ending</t>
   </si>
   <si>
     <t>ALTERNATE CRUISE</t>
@@ -425,6 +632,12 @@
     <t>Speed (TAS) at alternate cruise ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at alternate cruise ending</t>
+  </si>
+  <si>
     <t>Mach at alternate cruise start</t>
   </si>
   <si>
@@ -461,6 +674,30 @@
     <t>Drag at alternate cruise ending</t>
   </si>
   <si>
+    <t>Rate of climb at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Rate of climb at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Climb angle at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Climb angle at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Fuel flow at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>SFC at alternate cruise start</t>
+  </si>
+  <si>
+    <t>SFC at alternate cruise ending</t>
+  </si>
+  <si>
     <t>SECOND DESCENT</t>
   </si>
   <si>
@@ -470,6 +707,12 @@
     <t>Speed (TAS) at second descent ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at second descent start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at second descent ending</t>
+  </si>
+  <si>
     <t>Mach at second descent start</t>
   </si>
   <si>
@@ -506,6 +749,30 @@
     <t>Drag at second descent ending</t>
   </si>
   <si>
+    <t>Rate of climb at second descent start</t>
+  </si>
+  <si>
+    <t>Rate of climb at second descent ending</t>
+  </si>
+  <si>
+    <t>Climb angle at second descent start</t>
+  </si>
+  <si>
+    <t>Climb angle at second descent ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at second descent start</t>
+  </si>
+  <si>
+    <t>Fuel flow at second descent ending</t>
+  </si>
+  <si>
+    <t>SFC at second descent start</t>
+  </si>
+  <si>
+    <t>SFC at second descent ending</t>
+  </si>
+  <si>
     <t>HOLDING</t>
   </si>
   <si>
@@ -515,6 +782,12 @@
     <t>Speed (TAS) at holding ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at holding start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at holding ending</t>
+  </si>
+  <si>
     <t>Mach at holding start</t>
   </si>
   <si>
@@ -551,6 +824,30 @@
     <t>Drag at holding ending</t>
   </si>
   <si>
+    <t>Rate of climb at holding start</t>
+  </si>
+  <si>
+    <t>Rate of climb at holding ending</t>
+  </si>
+  <si>
+    <t>Climb angle at holding start</t>
+  </si>
+  <si>
+    <t>Climb angle at holding ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at holding start</t>
+  </si>
+  <si>
+    <t>Fuel flow at holding ending</t>
+  </si>
+  <si>
+    <t>SFC at holding start</t>
+  </si>
+  <si>
+    <t>SFC at holding ending</t>
+  </si>
+  <si>
     <t>THIRD DESCENT</t>
   </si>
   <si>
@@ -560,6 +857,12 @@
     <t>Speed (TAS) at third descent ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at third descent start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at third descent ending</t>
+  </si>
+  <si>
     <t>Mach at third descent start</t>
   </si>
   <si>
@@ -596,6 +899,30 @@
     <t>Drag at third descent ending</t>
   </si>
   <si>
+    <t>Rate of climb at third descent start</t>
+  </si>
+  <si>
+    <t>Rate of climb at third descent ending</t>
+  </si>
+  <si>
+    <t>Climb angle at third descent start</t>
+  </si>
+  <si>
+    <t>Climb angle at third descent ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at third descent start</t>
+  </si>
+  <si>
+    <t>Fuel flow at third descent ending</t>
+  </si>
+  <si>
+    <t>SFC at third descent start</t>
+  </si>
+  <si>
+    <t>SFC at third descent ending</t>
+  </si>
+  <si>
     <t>LANDING</t>
   </si>
   <si>
@@ -605,6 +932,12 @@
     <t>Speed (TAS) at landing ending</t>
   </si>
   <si>
+    <t>Speed (CAS) at landing start</t>
+  </si>
+  <si>
+    <t>Speed (CAS) at landing ending</t>
+  </si>
+  <si>
     <t>Mach at landing start</t>
   </si>
   <si>
@@ -639,6 +972,30 @@
   </si>
   <si>
     <t>Drag at landing ending</t>
+  </si>
+  <si>
+    <t>Rate of climb at landing start</t>
+  </si>
+  <si>
+    <t>Rate of climb at landing ending</t>
+  </si>
+  <si>
+    <t>Climb angle at landing start</t>
+  </si>
+  <si>
+    <t>Climb angle at landing ending</t>
+  </si>
+  <si>
+    <t>Fuel flow at landing start</t>
+  </si>
+  <si>
+    <t>Fuel flow at landing ending</t>
+  </si>
+  <si>
+    <t>SFC at landing start</t>
+  </si>
+  <si>
+    <t>SFC at landing ending</t>
   </si>
 </sst>
 </file>
@@ -729,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>499.9999999999999</v>
+        <v>1599.9999999999995</v>
       </c>
     </row>
     <row r="3">
@@ -737,43 +1094,43 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>112.84340945255747</v>
+        <v>1699.9999999999989</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="n">
-        <v>52263.1431262652</v>
+        <v>219.6262358374561</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>49919.610559671804</v>
+        <v>268.24341977860956</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" t="n">
-        <v>2467.1431262652072</v>
+        <v>59255.69365512255</v>
       </c>
     </row>
     <row r="7">
@@ -781,10 +1138,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>2343.7859699519468</v>
+        <v>49415.79102763352</v>
       </c>
     </row>
     <row r="8">
@@ -792,46 +1149,54 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>5.0</v>
+        <v>9459.693655122557</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9"/>
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7599.924283986242</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>130.0</v>
+        <v>8986.708972366428</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
       <c r="C12" t="n">
-        <v>0.5308083423660894</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="13">
@@ -839,21 +1204,15 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C13" t="n">
-        <v>96.57603827332888</v>
+        <v>130.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="n">
-        <v>142.887868983031</v>
       </c>
     </row>
     <row r="15">
@@ -864,7 +1223,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>95.44884708572306</v>
+        <v>0.6475561876113012</v>
       </c>
     </row>
     <row r="16">
@@ -875,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>22.017503337030206</v>
+        <v>139.23555376306024</v>
       </c>
     </row>
     <row r="17">
@@ -886,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>100.0</v>
+        <v>1346.7215767558046</v>
       </c>
     </row>
     <row r="18">
@@ -897,7 +1256,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>38.39482262187991</v>
+        <v>112.84256831326559</v>
       </c>
     </row>
     <row r="19">
@@ -908,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>26.10371062354659</v>
       </c>
     </row>
     <row r="20">
@@ -919,7 +1278,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>3.586709101989584</v>
+        <v>24.257438428022624</v>
       </c>
     </row>
     <row r="21">
@@ -930,45 +1289,45 @@
         <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5573494361384519</v>
+        <v>45.397348870165274</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-1.1368683772161603E-13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4023727896790188</v>
+        <v>4.2415020782649435</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>16.40161372463008</v>
+        <v>0.5527449802578985</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="n">
-        <v>18.64913214034498</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
@@ -976,437 +1335,443 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C26" t="n">
-        <v>18.999999999999993</v>
+        <v>34.999999999999986</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
       <c r="C27" t="n">
-        <v>4.476945800608419</v>
+        <v>29999.999999999993</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C28" t="n">
-        <v>13.595467385791132</v>
+        <v>29999.999999999993</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C29" t="n">
-        <v>8.999999999999986</v>
+        <v>1500.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C30" t="n">
-        <v>29.999999999999986</v>
+        <v>14999.999999999996</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C31" t="n">
-        <v>0.9666666666666615</v>
+        <v>14999.999999999996</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3512109448371987</v>
+        <v>1500.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1500.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>37.33126781772375</v>
+        <v>49.99999999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C35" t="n">
-        <v>788.8369109468399</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" t="n">
-        <v>537.6088759926045</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" t="n">
-        <v>1.5680932681558488</v>
+        <v>0.4729967210266096</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" t="n">
-        <v>270.00861556829545</v>
+        <v>24.05205605485038</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" t="n">
-        <v>564.3780993874409</v>
+        <v>175.75213189107245</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" t="n">
-        <v>21.583618213096315</v>
+        <v>18.999999999999986</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" t="n">
-        <v>122.50075931938022</v>
+        <v>5.499500051565391</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.03027056158975938</v>
+        <v>3.15101722292151</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>8.999999999999986</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="n">
+        <v>29.99999999999997</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" t="n">
-        <v>52226.065261806056</v>
+        <v>0.9666666666666117</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" t="n">
-        <v>51437.228350859215</v>
+        <v>0.3490511705066126</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" t="n">
-        <v>50899.6194748666</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C48" t="n">
-        <v>50898.051381598445</v>
+        <v>43.93750977125792</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>50628.04276603015</v>
+        <v>1107.2657272479946</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C50" t="n">
-        <v>50063.664666642704</v>
+        <v>6391.366013090939</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C51" t="n">
-        <v>50042.08104842961</v>
+        <v>57.35503387605013</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C52" t="n">
-        <v>49919.58028911022</v>
+        <v>330.19563717111396</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C53" t="n">
-        <v>49919.61055967181</v>
+        <v>169.2815470139135</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C54" t="n">
-        <v>49919.610559671804</v>
+        <v>5.275796573162097</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>59</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" t="n">
+        <v>875.8414607545983</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="n">
+        <v>6.190246867400674</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0</v>
+        <v>-9.094947017729282E-13</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" t="n">
-        <v>147.06581114238537</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0</v>
+        <v>58358.56249022873</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2223556780512614</v>
+        <v>57251.29676298074</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C61" t="n">
-        <v>1.4143</v>
+        <v>50859.93074988979</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>2.126695251478622</v>
+        <v>50802.57571601373</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>0.07121541061107992</v>
+        <v>58028.36685305761</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>0.09267083118915845</v>
+        <v>50303.0985318287</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C65" t="n">
-        <v>19.859465639027835</v>
+        <v>50297.82273525553</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>22.94891741218594</v>
+        <v>49421.981274500926</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C67" t="n">
-        <v>46611.9489095388</v>
+        <v>49415.791027633524</v>
       </c>
     </row>
     <row r="68">
@@ -1414,1508 +1779,2750 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C68" t="n">
-        <v>37403.91950088453</v>
+        <v>49415.79102763352</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" t="n">
-        <v>0.0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" t="n">
-        <v>7022.615112008484</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" t="n">
+        <v>6.424466346461113E-4</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
         <v>74</v>
+      </c>
+      <c r="C72" t="n">
+        <v>152.0394043271288</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C73" t="n">
-        <v>259.9999999999999</v>
+        <v>6.42117706590054E-4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C74" t="n">
-        <v>424.73295727057376</v>
+        <v>151.96156124567665</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C75" t="n">
-        <v>0.3930588576732219</v>
+        <v>9.712282320384863E-7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7205798230090309</v>
+        <v>0.22987548619942474</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C77" t="n">
-        <v>0.41383800477273924</v>
+        <v>1.4143</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C78" t="n">
-        <v>1.0876918253545205</v>
+        <v>2.1261710818515493</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C79" t="n">
-        <v>0.029563764164287156</v>
+        <v>0.0764434613177715</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C80" t="n">
-        <v>0.07332278232273193</v>
+        <v>0.12743665027045256</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C81" t="n">
-        <v>13.9981499809369</v>
+        <v>18.5012553803762</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C82" t="n">
-        <v>14.83429557496904</v>
+        <v>16.68414131522824</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C83" t="n">
-        <v>24073.62015582046</v>
+        <v>46611.95422864479</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C84" t="n">
-        <v>11059.118118010332</v>
+        <v>37137.38778182301</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" t="s">
         <v>87</v>
       </c>
-      <c r="B85" t="s">
-        <v>70</v>
-      </c>
       <c r="C85" t="n">
-        <v>8221.467394931173</v>
+        <v>1.048822531708138E-7</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C86" t="n">
-        <v>7807.31702248335</v>
+        <v>8210.337913343</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>91</v>
+      </c>
+      <c r="B87" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="B88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1670.1520318251498</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B89" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C89" t="n">
-        <v>459.08300177402543</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B90" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C90" t="n">
-        <v>460.52731432613206</v>
+        <v>6.227347510862037</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C91" t="n">
-        <v>0.7788563201937818</v>
+        <v>11593.656426747557</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C92" t="n">
-        <v>0.7813066656763994</v>
+        <v>12646.303280799812</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B93" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C93" t="n">
-        <v>0.348875229484687</v>
+        <v>0.24872710485120192</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B94" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C94" t="n">
-        <v>0.34125228922845885</v>
+        <v>0.34052753939224495</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>96</v>
-      </c>
-      <c r="B95" t="s">
-        <v>17</v>
-      </c>
-      <c r="C95" t="n">
-        <v>0.025547831227245296</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>97</v>
-      </c>
-      <c r="B96" t="s">
-        <v>17</v>
-      </c>
-      <c r="C96" t="n">
-        <v>0.025369749949183916</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C97" t="n">
-        <v>13.655766956556047</v>
+        <v>250.12806376957104</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B98" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C98" t="n">
-        <v>13.45114910127193</v>
+        <v>408.39707429862864</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C99" t="n">
-        <v>8304.160256122626</v>
+        <v>249.99999999999994</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B100" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C100" t="n">
-        <v>8298.244601761078</v>
+        <v>249.99999999999994</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B101" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C101" t="n">
-        <v>8304.160256122626</v>
+        <v>0.3781348116049325</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C102" t="n">
-        <v>8298.244601761078</v>
+        <v>0.6928652144317605</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>17</v>
+        <v>110</v>
+      </c>
+      <c r="B103" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0.4996541553043212</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>111</v>
+      </c>
+      <c r="B104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0.49067630386272</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B105" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C105" t="n">
-        <v>359.38939993419694</v>
+        <v>0.032879869593364225</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C106" t="n">
-        <v>250.550253192183</v>
+        <v>0.032472882303399106</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B107" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C107" t="n">
-        <v>0.6097213455251858</v>
+        <v>15.196354531927973</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B108" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C108" t="n">
-        <v>0.3807413742403091</v>
+        <v>15.110340353475747</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B109" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C109" t="n">
-        <v>0.5628463321985737</v>
+        <v>24545.39587485186</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B110" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C110" t="n">
-        <v>0.5625034934743327</v>
+        <v>11052.127404856908</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B111" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C111" t="n">
-        <v>0.03247844996867854</v>
+        <v>8461.083779376106</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B112" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C112" t="n">
-        <v>0.03246436440058862</v>
+        <v>9164.674773252658</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B113" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C113" t="n">
-        <v>17.329839716531104</v>
+        <v>3164.836459141452</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B114" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C114" t="n">
-        <v>17.326798286681804</v>
+        <v>451.83160671283474</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B115" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C115" t="n">
-        <v>-311.0648126141039</v>
+        <v>7.177720991556505</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B116" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C116" t="n">
-        <v>809.9170717580963</v>
+        <v>0.6259871462212071</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B117" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C117" t="n">
-        <v>7120.31593457726</v>
+        <v>9736.241507263418</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B118" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C118" t="n">
-        <v>7117.22002628589</v>
+        <v>4689.162044776636</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>126</v>
+      </c>
+      <c r="B119" t="s">
+        <v>101</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0.3966626391729434</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>127</v>
+      </c>
+      <c r="B120" t="s">
+        <v>101</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0.42427687204510167</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>120</v>
-      </c>
-      <c r="B121" t="s">
-        <v>59</v>
-      </c>
-      <c r="C121" t="n">
-        <v>265.79895987241326</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>121</v>
-      </c>
-      <c r="B122" t="s">
-        <v>59</v>
-      </c>
-      <c r="C122" t="n">
-        <v>327.7100016954031</v>
+        <v>128</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B123" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C123" t="n">
-        <v>0.4039136259656544</v>
+        <v>459.7571234892813</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B124" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C124" t="n">
-        <v>0.523108958484267</v>
+        <v>459.7571234892813</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B125" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C125" t="n">
-        <v>0.40331486984889353</v>
+        <v>459.7571309454785</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C126" t="n">
-        <v>0.6098275704612877</v>
+        <v>459.7571309454785</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B127" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C127" t="n">
-        <v>0.029169799947729794</v>
+        <v>0.7799999999999998</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B128" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C128" t="n">
-        <v>0.03814301431355167</v>
+        <v>0.7799999999999998</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B129" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C129" t="n">
-        <v>13.826453063497352</v>
+        <v>0.38717151307515857</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B130" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C130" t="n">
-        <v>15.987922859170169</v>
+        <v>0.32114642513884273</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C131" t="n">
-        <v>23411.656515649072</v>
+        <v>0.026595971757839246</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B132" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C132" t="n">
-        <v>17388.51972278026</v>
+        <v>0.024900052187787732</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B133" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C133" t="n">
-        <v>7946.904670725951</v>
+        <v>14.557524598101535</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B134" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C134" t="n">
-        <v>6968.1702634312605</v>
+        <v>12.897419761085862</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>141</v>
+      </c>
+      <c r="B135" t="s">
+        <v>87</v>
+      </c>
+      <c r="C135" t="n">
+        <v>8670.258677790936</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>142</v>
+      </c>
+      <c r="B136" t="s">
+        <v>87</v>
+      </c>
+      <c r="C136" t="n">
+        <v>8117.390690752993</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B137" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C137" t="n">
-        <v>441.21068121021403</v>
+        <v>8670.258677790936</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B138" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C138" t="n">
-        <v>441.21068121021403</v>
+        <v>8117.390690752993</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B139" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C139" t="n">
-        <v>0.704285065228287</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B140" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C140" t="n">
-        <v>0.704285065228287</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B141" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C141" t="n">
-        <v>0.22132046496662092</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B142" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C142" t="n">
-        <v>0.217171901093037</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C143" t="n">
-        <v>0.022849750062349312</v>
+        <v>4946.385159359811</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C144" t="n">
-        <v>0.022772084157704518</v>
+        <v>4630.973808003639</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B145" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C145" t="n">
-        <v>9.685903100152585</v>
+        <v>0.5705002979934253</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B146" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C146" t="n">
-        <v>9.536759990392046</v>
+        <v>0.5705002979934253</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>145</v>
-      </c>
-      <c r="B147" t="s">
-        <v>70</v>
-      </c>
-      <c r="C147" t="n">
-        <v>11523.52312714743</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>146</v>
-      </c>
-      <c r="B148" t="s">
-        <v>70</v>
-      </c>
-      <c r="C148" t="n">
-        <v>11507.889093627313</v>
+        <v>153</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B149" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C149" t="n">
-        <v>11523.52312714743</v>
+        <v>424.73292719496004</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B150" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C150" t="n">
-        <v>11507.889093627313</v>
+        <v>296.1048446816708</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>156</v>
+      </c>
+      <c r="B151" t="s">
+        <v>74</v>
+      </c>
+      <c r="C151" t="n">
+        <v>259.9999999999999</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>149</v>
+        <v>157</v>
+      </c>
+      <c r="B152" t="s">
+        <v>74</v>
+      </c>
+      <c r="C152" t="n">
+        <v>259.9999999999999</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B153" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C153" t="n">
-        <v>277.2930587223476</v>
+        <v>0.7205797719843104</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B154" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C154" t="n">
-        <v>236.549695229041</v>
+        <v>0.44996707864763796</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B155" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C155" t="n">
-        <v>0.44263062583603374</v>
+        <v>0.402767715515767</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B156" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C156" t="n">
-        <v>0.35946583525720144</v>
+        <v>0.4008550483052877</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B157" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C157" t="n">
-        <v>0.5532821109211329</v>
+        <v>0.029149315631055522</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B158" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C158" t="n">
-        <v>0.5525422808074715</v>
+        <v>0.029077709361197294</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B159" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C159" t="n">
-        <v>0.03209357219044354</v>
+        <v>13.817398686597652</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B160" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C160" t="n">
-        <v>0.03206645570595816</v>
+        <v>13.785647394915092</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B161" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C161" t="n">
-        <v>17.23965495763301</v>
+        <v>4114.730957686313</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B162" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C162" t="n">
-        <v>17.231161618675724</v>
+        <v>-428.4840628147698</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B163" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C163" t="n">
-        <v>1131.8962165037506</v>
+        <v>8109.974379657993</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B164" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C164" t="n">
-        <v>445.58197273788926</v>
+        <v>8090.051956046978</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B165" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C165" t="n">
-        <v>7033.948934994985</v>
+        <v>-1532.5827082670585</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B166" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C166" t="n">
-        <v>7027.268108060516</v>
+        <v>-2287.508507424009</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>17</v>
+        <v>172</v>
+      </c>
+      <c r="B167" t="s">
+        <v>95</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1.9985327130221981</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>164</v>
+        <v>173</v>
+      </c>
+      <c r="B168" t="s">
+        <v>95</v>
+      </c>
+      <c r="C168" t="n">
+        <v>2.867311648707845</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B169" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C169" t="n">
-        <v>197.41767258058383</v>
+        <v>2020.2986441137873</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B170" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="C170" t="n">
-        <v>197.41767258058383</v>
+        <v>-225.85383695675415</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B171" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C171" t="n">
-        <v>0.29999999999999993</v>
+        <v>0.4909916747630539</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B172" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="C172" t="n">
-        <v>0.29999999999999993</v>
+        <v>0.5270997373229933</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>169</v>
-      </c>
-      <c r="B173" t="s">
-        <v>17</v>
-      </c>
-      <c r="C173" t="n">
-        <v>0.7188080623029574</v>
+        <v>20</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>170</v>
-      </c>
-      <c r="B174" t="s">
-        <v>17</v>
-      </c>
-      <c r="C174" t="n">
-        <v>0.717487619075011</v>
+        <v>178</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B175" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C175" t="n">
-        <v>0.0394401926933973</v>
+        <v>250.1829793709091</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B176" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C176" t="n">
-        <v>0.03937423095146737</v>
+        <v>408.39707429862864</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B177" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C177" t="n">
-        <v>18.22526750543218</v>
+        <v>249.99999999999994</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B178" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C178" t="n">
-        <v>18.22226369219466</v>
+        <v>249.99999999999994</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B179" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C179" t="n">
-        <v>6053.34895034462</v>
+        <v>0.38018325730507274</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B180" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C180" t="n">
-        <v>6043.225028172676</v>
+        <v>0.6519061581249693</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B181" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C181" t="n">
-        <v>6053.34895034462</v>
+        <v>0.4994348294570125</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B182" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C182" t="n">
-        <v>6043.225028172676</v>
+        <v>0.4973362382432412</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>17</v>
+        <v>187</v>
+      </c>
+      <c r="B183" t="s">
+        <v>20</v>
+      </c>
+      <c r="C183" t="n">
+        <v>0.032869927032742</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>179</v>
+        <v>188</v>
+      </c>
+      <c r="B184" t="s">
+        <v>20</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0.032774792917815605</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="B185" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C185" t="n">
-        <v>224.90679627393837</v>
+        <v>15.194278617032568</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="B186" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C186" t="n">
-        <v>221.33361546517457</v>
+        <v>15.174351810256624</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B187" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C187" t="n">
-        <v>0.3417730439236138</v>
+        <v>23870.88892579321</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="B188" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C188" t="n">
-        <v>0.3346619068734856</v>
+        <v>17683.041611604847</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B189" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C189" t="n">
-        <v>0.5512790648823496</v>
+        <v>8350.275645298701</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B190" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C190" t="n">
-        <v>0.5512413716588563</v>
+        <v>7987.563558698754</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="B191" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C191" t="n">
-        <v>0.03202015592117955</v>
+        <v>3053.8146328529174</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B192" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C192" t="n">
-        <v>0.03201877437737485</v>
+        <v>963.2678782933895</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B193" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C193" t="n">
-        <v>17.21662649736534</v>
+        <v>1.3347338026948294</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B194" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C194" t="n">
-        <v>17.216192136585192</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="B195" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C195" t="n">
-        <v>-58.59660992986095</v>
+        <v>9413.461735757806</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B196" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="C196" t="n">
-        <v>13.594577309080737</v>
+        <v>6839.387827971675</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B197" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C197" t="n">
-        <v>7015.860993344899</v>
+        <v>0.3943490234075983</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="B198" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C198" t="n">
-        <v>7015.520615333634</v>
+        <v>0.3867766630986827</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B201" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C201" t="n">
-        <v>117.3037566830413</v>
+        <v>461.897286721882</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B202" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C202" t="n">
-        <v>0.0</v>
+        <v>461.897286721882</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="B203" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C203" t="n">
-        <v>0.17736618458277903</v>
+        <v>366.462097361656</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B204" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C204" t="n">
-        <v>0.0</v>
+        <v>366.462097361656</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="B205" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C205" t="n">
-        <v>1.946133482233357</v>
+        <v>0.7373061772108307</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B206" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C206" t="n">
-        <v>2.0027</v>
+        <v>0.7373061772108307</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B207" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C207" t="n">
-        <v>0.10563975337709984</v>
+        <v>0.20131931017031487</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B208" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C208" t="n">
-        <v>0.10773409853304787</v>
+        <v>0.200306306109778</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B209" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C209" t="n">
-        <v>18.42235919735905</v>
+        <v>0.0225421143988641</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B210" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C210" t="n">
-        <v>18.58928628233394</v>
+        <v>0.02252741899035696</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="B211" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C211" t="n">
-        <v>0.0</v>
+        <v>8.930808645903216</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="B212" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C212" t="n">
-        <v>0.0</v>
+        <v>8.891666914683867</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B213" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C213" t="n">
-        <v>4558.735009648629</v>
+        <v>12459.403768706807</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B214" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C214" t="n">
+        <v>12451.281370563633</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>218</v>
+      </c>
+      <c r="B215" t="s">
+        <v>87</v>
+      </c>
+      <c r="C215" t="n">
+        <v>12459.403768706807</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>219</v>
+      </c>
+      <c r="B216" t="s">
+        <v>87</v>
+      </c>
+      <c r="C216" t="n">
+        <v>12451.281370563633</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>220</v>
+      </c>
+      <c r="B217" t="s">
+        <v>92</v>
+      </c>
+      <c r="C217" t="n">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>221</v>
+      </c>
+      <c r="B218" t="s">
+        <v>92</v>
+      </c>
+      <c r="C218" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>222</v>
+      </c>
+      <c r="B219" t="s">
+        <v>95</v>
+      </c>
+      <c r="C219" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>223</v>
+      </c>
+      <c r="B220" t="s">
+        <v>95</v>
+      </c>
+      <c r="C220" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>224</v>
+      </c>
+      <c r="B221" t="s">
+        <v>98</v>
+      </c>
+      <c r="C221" t="n">
+        <v>7108.093562867635</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>225</v>
+      </c>
+      <c r="B222" t="s">
+        <v>98</v>
+      </c>
+      <c r="C222" t="n">
+        <v>7103.459732306535</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>226</v>
+      </c>
+      <c r="B223" t="s">
+        <v>101</v>
+      </c>
+      <c r="C223" t="n">
+        <v>0.5705002979934249</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>227</v>
+      </c>
+      <c r="B224" t="s">
+        <v>101</v>
+      </c>
+      <c r="C224" t="n">
+        <v>0.5705002979934252</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>229</v>
+      </c>
+      <c r="B227" t="s">
+        <v>74</v>
+      </c>
+      <c r="C227" t="n">
+        <v>327.7099784900472</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228" t="s">
+        <v>74</v>
+      </c>
+      <c r="C228" t="n">
+        <v>279.55873072523025</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>231</v>
+      </c>
+      <c r="B229" t="s">
+        <v>74</v>
+      </c>
+      <c r="C229" t="n">
+        <v>259.9999999999999</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>232</v>
+      </c>
+      <c r="B230" t="s">
+        <v>74</v>
+      </c>
+      <c r="C230" t="n">
+        <v>259.9999999999999</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>233</v>
+      </c>
+      <c r="B231" t="s">
+        <v>20</v>
+      </c>
+      <c r="C231" t="n">
+        <v>0.5231089214425853</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>234</v>
+      </c>
+      <c r="B232" t="s">
+        <v>20</v>
+      </c>
+      <c r="C232" t="n">
+        <v>0.42482325984941977</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>235</v>
+      </c>
+      <c r="B233" t="s">
+        <v>20</v>
+      </c>
+      <c r="C233" t="n">
+        <v>0.39819317017962225</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>236</v>
+      </c>
+      <c r="B234" t="s">
+        <v>20</v>
+      </c>
+      <c r="C234" t="n">
+        <v>0.39818889157485216</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>237</v>
+      </c>
+      <c r="B235" t="s">
+        <v>20</v>
+      </c>
+      <c r="C235" t="n">
+        <v>0.02897805419779417</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>238</v>
+      </c>
+      <c r="B236" t="s">
+        <v>20</v>
+      </c>
+      <c r="C236" t="n">
+        <v>0.028977894015758267</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>239</v>
+      </c>
+      <c r="B237" t="s">
+        <v>20</v>
+      </c>
+      <c r="C237" t="n">
+        <v>13.74119764776798</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>240</v>
+      </c>
+      <c r="B238" t="s">
+        <v>20</v>
+      </c>
+      <c r="C238" t="n">
+        <v>13.7411259547818</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>241</v>
+      </c>
+      <c r="B239" t="s">
+        <v>87</v>
+      </c>
+      <c r="C239" t="n">
+        <v>-458.06770088098824</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>242</v>
+      </c>
+      <c r="B240" t="s">
+        <v>87</v>
+      </c>
+      <c r="C240" t="n">
+        <v>2286.23591205904</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>243</v>
+      </c>
+      <c r="B241" t="s">
+        <v>87</v>
+      </c>
+      <c r="C241" t="n">
+        <v>8062.32571944405</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>244</v>
+      </c>
+      <c r="B242" t="s">
+        <v>87</v>
+      </c>
+      <c r="C242" t="n">
+        <v>8062.281153313457</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>245</v>
+      </c>
+      <c r="B243" t="s">
+        <v>92</v>
+      </c>
+      <c r="C243" t="n">
+        <v>-2549.73524023793</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>246</v>
+      </c>
+      <c r="B244" t="s">
+        <v>92</v>
+      </c>
+      <c r="C244" t="n">
+        <v>-1473.9668084606797</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>247</v>
+      </c>
+      <c r="B245" t="s">
+        <v>95</v>
+      </c>
+      <c r="C245" t="n">
+        <v>2.5905825739873594</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>248</v>
+      </c>
+      <c r="B246" t="s">
+        <v>95</v>
+      </c>
+      <c r="C246" t="n">
+        <v>3.037172576791759</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>249</v>
+      </c>
+      <c r="B247" t="s">
+        <v>98</v>
+      </c>
+      <c r="C247" t="n">
+        <v>-159.14691502766723</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>250</v>
+      </c>
+      <c r="B248" t="s">
+        <v>98</v>
+      </c>
+      <c r="C248" t="n">
+        <v>896.0747022210725</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>251</v>
+      </c>
+      <c r="B249" t="s">
+        <v>101</v>
+      </c>
+      <c r="C249" t="n">
+        <v>0.34743099048805365</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>252</v>
+      </c>
+      <c r="B250" t="s">
+        <v>101</v>
+      </c>
+      <c r="C250" t="n">
+        <v>0.3919432362577341</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>254</v>
+      </c>
+      <c r="B253" t="s">
+        <v>74</v>
+      </c>
+      <c r="C253" t="n">
+        <v>195.1355835079958</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>255</v>
+      </c>
+      <c r="B254" t="s">
+        <v>74</v>
+      </c>
+      <c r="C254" t="n">
+        <v>195.1355835079958</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>256</v>
+      </c>
+      <c r="B255" t="s">
+        <v>74</v>
+      </c>
+      <c r="C255" t="n">
+        <v>190.87829288885263</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>257</v>
+      </c>
+      <c r="B256" t="s">
+        <v>74</v>
+      </c>
+      <c r="C256" t="n">
+        <v>190.87829288885263</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>258</v>
+      </c>
+      <c r="B257" t="s">
+        <v>20</v>
+      </c>
+      <c r="C257" t="n">
+        <v>0.29653208999565644</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>259</v>
+      </c>
+      <c r="B258" t="s">
+        <v>20</v>
+      </c>
+      <c r="C258" t="n">
+        <v>0.29653208999565644</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>260</v>
+      </c>
+      <c r="B259" t="s">
+        <v>20</v>
+      </c>
+      <c r="C259" t="n">
+        <v>0.7394790522448984</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>261</v>
+      </c>
+      <c r="B260" t="s">
+        <v>20</v>
+      </c>
+      <c r="C260" t="n">
+        <v>0.7200226046573762</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>262</v>
+      </c>
+      <c r="B261" t="s">
+        <v>20</v>
+      </c>
+      <c r="C261" t="n">
+        <v>0.045637069649689596</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>263</v>
+      </c>
+      <c r="B262" t="s">
+        <v>20</v>
+      </c>
+      <c r="C262" t="n">
+        <v>0.04444670248359444</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>264</v>
+      </c>
+      <c r="B263" t="s">
+        <v>20</v>
+      </c>
+      <c r="C263" t="n">
+        <v>16.203473577973867</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>265</v>
+      </c>
+      <c r="B264" t="s">
+        <v>20</v>
+      </c>
+      <c r="C264" t="n">
+        <v>16.199685565495912</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>266</v>
+      </c>
+      <c r="B265" t="s">
+        <v>87</v>
+      </c>
+      <c r="C265" t="n">
+        <v>6843.453491516708</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>267</v>
+      </c>
+      <c r="B266" t="s">
+        <v>87</v>
+      </c>
+      <c r="C266" t="n">
+        <v>6664.953373048735</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>268</v>
+      </c>
+      <c r="B267" t="s">
+        <v>87</v>
+      </c>
+      <c r="C267" t="n">
+        <v>6843.453491516708</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>269</v>
+      </c>
+      <c r="B268" t="s">
+        <v>87</v>
+      </c>
+      <c r="C268" t="n">
+        <v>6664.953373048735</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>270</v>
+      </c>
+      <c r="B269" t="s">
+        <v>92</v>
+      </c>
+      <c r="C269" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>271</v>
+      </c>
+      <c r="B270" t="s">
+        <v>92</v>
+      </c>
+      <c r="C270" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>272</v>
+      </c>
+      <c r="B271" t="s">
+        <v>95</v>
+      </c>
+      <c r="C271" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>273</v>
+      </c>
+      <c r="B272" t="s">
+        <v>95</v>
+      </c>
+      <c r="C272" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>274</v>
+      </c>
+      <c r="B273" t="s">
+        <v>98</v>
+      </c>
+      <c r="C273" t="n">
+        <v>3904.192256214428</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>275</v>
+      </c>
+      <c r="B274" t="s">
+        <v>98</v>
+      </c>
+      <c r="C274" t="n">
+        <v>3802.357885436587</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>276</v>
+      </c>
+      <c r="B275" t="s">
+        <v>101</v>
+      </c>
+      <c r="C275" t="n">
+        <v>0.5705002979934253</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>277</v>
+      </c>
+      <c r="B276" t="s">
+        <v>101</v>
+      </c>
+      <c r="C276" t="n">
+        <v>0.570500297993425</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>279</v>
+      </c>
+      <c r="B279" t="s">
+        <v>74</v>
+      </c>
+      <c r="C279" t="n">
+        <v>265.798941051018</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>280</v>
+      </c>
+      <c r="B280" t="s">
+        <v>74</v>
+      </c>
+      <c r="C280" t="n">
+        <v>261.5760910042972</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>281</v>
+      </c>
+      <c r="B281" t="s">
+        <v>74</v>
+      </c>
+      <c r="C281" t="n">
+        <v>259.9999999999999</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>282</v>
+      </c>
+      <c r="B282" t="s">
+        <v>74</v>
+      </c>
+      <c r="C282" t="n">
+        <v>259.9999999999999</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>283</v>
+      </c>
+      <c r="B283" t="s">
+        <v>20</v>
+      </c>
+      <c r="C283" t="n">
+        <v>0.4039135973642708</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>284</v>
+      </c>
+      <c r="B284" t="s">
+        <v>20</v>
+      </c>
+      <c r="C284" t="n">
+        <v>0.39550952630502845</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>285</v>
+      </c>
+      <c r="B285" t="s">
+        <v>20</v>
+      </c>
+      <c r="C285" t="n">
+        <v>0.3910100316573717</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>286</v>
+      </c>
+      <c r="B286" t="s">
+        <v>20</v>
+      </c>
+      <c r="C286" t="n">
+        <v>0.39091567612387257</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>287</v>
+      </c>
+      <c r="B287" t="s">
+        <v>20</v>
+      </c>
+      <c r="C287" t="n">
+        <v>0.02875728285691221</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>288</v>
+      </c>
+      <c r="B288" t="s">
+        <v>20</v>
+      </c>
+      <c r="C288" t="n">
+        <v>0.02875449338496759</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>289</v>
+      </c>
+      <c r="B289" t="s">
+        <v>20</v>
+      </c>
+      <c r="C289" t="n">
+        <v>13.596904603363354</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>290</v>
+      </c>
+      <c r="B290" t="s">
+        <v>20</v>
+      </c>
+      <c r="C290" t="n">
+        <v>13.594942219647566</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>291</v>
+      </c>
+      <c r="B291" t="s">
+        <v>87</v>
+      </c>
+      <c r="C291" t="n">
+        <v>2228.0037723703</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>292</v>
+      </c>
+      <c r="B292" t="s">
+        <v>87</v>
+      </c>
+      <c r="C292" t="n">
+        <v>2120.567491498331</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>293</v>
+      </c>
+      <c r="B293" t="s">
+        <v>87</v>
+      </c>
+      <c r="C293" t="n">
+        <v>8000.9023247758105</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>294</v>
+      </c>
+      <c r="B294" t="s">
+        <v>87</v>
+      </c>
+      <c r="C294" t="n">
+        <v>8000.126232935787</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>295</v>
+      </c>
+      <c r="B295" t="s">
+        <v>92</v>
+      </c>
+      <c r="C295" t="n">
+        <v>-1426.1576310578735</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>296</v>
+      </c>
+      <c r="B296" t="s">
+        <v>92</v>
+      </c>
+      <c r="C296" t="n">
+        <v>-1429.7033411410737</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>297</v>
+      </c>
+      <c r="B297" t="s">
+        <v>95</v>
+      </c>
+      <c r="C297" t="n">
+        <v>3.194558997631673</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>298</v>
+      </c>
+      <c r="B298" t="s">
+        <v>95</v>
+      </c>
+      <c r="C298" t="n">
+        <v>3.246186351024417</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>299</v>
+      </c>
+      <c r="B299" t="s">
+        <v>98</v>
+      </c>
+      <c r="C299" t="n">
+        <v>868.1939463532954</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>300</v>
+      </c>
+      <c r="B300" t="s">
+        <v>98</v>
+      </c>
+      <c r="C300" t="n">
+        <v>823.6176659102288</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>301</v>
+      </c>
+      <c r="B301" t="s">
+        <v>101</v>
+      </c>
+      <c r="C301" t="n">
+        <v>0.3896734633575833</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>302</v>
+      </c>
+      <c r="B302" t="s">
+        <v>101</v>
+      </c>
+      <c r="C302" t="n">
+        <v>0.3883949316455307</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>304</v>
+      </c>
+      <c r="B305" t="s">
+        <v>74</v>
+      </c>
+      <c r="C305" t="n">
+        <v>116.71030454427692</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>305</v>
+      </c>
+      <c r="B306" t="s">
+        <v>74</v>
+      </c>
+      <c r="C306" t="n">
+        <v>-1.770112286004983E-5</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>306</v>
+      </c>
+      <c r="B307" t="s">
+        <v>74</v>
+      </c>
+      <c r="C307" t="n">
+        <v>116.62494470821682</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>307</v>
+      </c>
+      <c r="B308" t="s">
+        <v>74</v>
+      </c>
+      <c r="C308" t="n">
+        <v>-1.76881765743614E-5</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>308</v>
+      </c>
+      <c r="B309" t="s">
+        <v>20</v>
+      </c>
+      <c r="C309" t="n">
+        <v>0.17646887025490512</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>309</v>
+      </c>
+      <c r="B310" t="s">
+        <v>20</v>
+      </c>
+      <c r="C310" t="n">
+        <v>-2.6759935118863632E-8</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>310</v>
+      </c>
+      <c r="B311" t="s">
+        <v>20</v>
+      </c>
+      <c r="C311" t="n">
+        <v>1.9461334822333567</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>311</v>
+      </c>
+      <c r="B312" t="s">
+        <v>20</v>
+      </c>
+      <c r="C312" t="n">
+        <v>2.0027</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>312</v>
+      </c>
+      <c r="B313" t="s">
+        <v>20</v>
+      </c>
+      <c r="C313" t="n">
+        <v>0.10563975337709984</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>313</v>
+      </c>
+      <c r="B314" t="s">
+        <v>20</v>
+      </c>
+      <c r="C314" t="n">
+        <v>0.10773409853304787</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>314</v>
+      </c>
+      <c r="B315" t="s">
+        <v>20</v>
+      </c>
+      <c r="C315" t="n">
+        <v>18.422359197359047</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>315</v>
+      </c>
+      <c r="B316" t="s">
+        <v>20</v>
+      </c>
+      <c r="C316" t="n">
+        <v>18.58928628233394</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>316</v>
+      </c>
+      <c r="B317" t="s">
+        <v>87</v>
+      </c>
+      <c r="C317" t="n">
+        <v>-5704.23887976628</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>317</v>
+      </c>
+      <c r="B318" t="s">
+        <v>87</v>
+      </c>
+      <c r="C318" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>318</v>
+      </c>
+      <c r="B319" t="s">
+        <v>87</v>
+      </c>
+      <c r="C319" t="n">
+        <v>5913.638400433003</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>319</v>
+      </c>
+      <c r="B320" t="s">
+        <v>87</v>
+      </c>
+      <c r="C320" t="n">
+        <v>1.3390009421019082E-10</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>320</v>
+      </c>
+      <c r="B321" t="s">
+        <v>92</v>
+      </c>
+      <c r="C321" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>321</v>
+      </c>
+      <c r="B322" t="s">
+        <v>92</v>
+      </c>
+      <c r="C322" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>322</v>
+      </c>
+      <c r="B323" t="s">
+        <v>95</v>
+      </c>
+      <c r="C323" t="n">
+        <v>-3.0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>323</v>
+      </c>
+      <c r="B324" t="s">
+        <v>95</v>
+      </c>
+      <c r="C324" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>324</v>
+      </c>
+      <c r="B325" t="s">
+        <v>98</v>
+      </c>
+      <c r="C325" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>325</v>
+      </c>
+      <c r="B326" t="s">
+        <v>98</v>
+      </c>
+      <c r="C326" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>326</v>
+      </c>
+      <c r="B327" t="s">
+        <v>101</v>
+      </c>
+      <c r="C327" t="n">
+        <v>-0.0</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>327</v>
+      </c>
+      <c r="B328" t="s">
+        <v>101</v>
+      </c>
+      <c r="C328" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on take-off calculator. More tests on ATR72 and CS300.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
+++ b/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
@@ -227,7 +227,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>282.14545254229256</v>
+        <v>282.1452529462797</v>
       </c>
     </row>
     <row r="4">
@@ -238,7 +238,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>151.46833787262005</v>
+        <v>151.46515118137688</v>
       </c>
     </row>
     <row r="5">
@@ -249,7 +249,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1427.3301750788414</v>
+        <v>1427.3267887915854</v>
       </c>
     </row>
     <row r="6">
@@ -260,7 +260,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1641.4297013406674</v>
+        <v>1641.4258071103227</v>
       </c>
     </row>
     <row r="7">
@@ -271,7 +271,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1822.627904700134</v>
+        <v>1853.2236402716744</v>
       </c>
     </row>
     <row r="8">
@@ -298,7 +298,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>925.6740568972853</v>
+        <v>925.6734020547234</v>
       </c>
     </row>
     <row r="11">
@@ -309,7 +309,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>496.94336572381917</v>
+        <v>496.93291070005546</v>
       </c>
     </row>
     <row r="12">
@@ -320,7 +320,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>4682.841781754729</v>
+        <v>4682.830671888403</v>
       </c>
     </row>
     <row r="13">
@@ -331,7 +331,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>5385.268049017937</v>
+        <v>5385.255272671663</v>
       </c>
     </row>
     <row r="14">
@@ -342,7 +342,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>5979.750343504376</v>
+        <v>6080.130053384759</v>
       </c>
     </row>
     <row r="15">
@@ -369,7 +369,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>63.08762052352435</v>
+        <v>63.5085873574696</v>
       </c>
     </row>
     <row r="18">
@@ -380,7 +380,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>68.17940572865422</v>
+        <v>68.3549361418386</v>
       </c>
     </row>
     <row r="19">
@@ -402,7 +402,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>74.32650167783808</v>
+        <v>74.326259768459</v>
       </c>
     </row>
     <row r="21">
@@ -413,7 +413,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="n">
-        <v>77.44662848321994</v>
+        <v>77.53034686818486</v>
       </c>
     </row>
     <row r="22">
@@ -440,7 +440,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>122.63252369583567</v>
+        <v>123.45081775750032</v>
       </c>
     </row>
     <row r="25">
@@ -451,7 +451,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="n">
-        <v>132.5301623235179</v>
+        <v>132.87136615044224</v>
       </c>
     </row>
     <row r="26">
@@ -473,7 +473,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="n">
-        <v>144.47916092884293</v>
+        <v>144.47869069462874</v>
       </c>
     </row>
     <row r="28">
@@ -484,7 +484,7 @@
         <v>19</v>
       </c>
       <c r="C28" t="n">
-        <v>150.54420223520077</v>
+        <v>150.70693775673084</v>
       </c>
     </row>
     <row r="29">
@@ -500,7 +500,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="n">
-        <v>0.9900900900900751</v>
+        <v>0.9966966966966815</v>
       </c>
     </row>
     <row r="31">
@@ -511,7 +511,7 @@
         <v>21</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0699999999999998</v>
+        <v>1.0727547547547536</v>
       </c>
     </row>
     <row r="32">
@@ -533,7 +533,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="n">
-        <v>1.1664718391914992</v>
+        <v>1.1664680426926468</v>
       </c>
     </row>
     <row r="34">
@@ -544,7 +544,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="n">
-        <v>1.2154387617699327</v>
+        <v>1.2167526287794068</v>
       </c>
     </row>
     <row r="35">
@@ -576,7 +576,7 @@
         <v>29</v>
       </c>
       <c r="C38" t="n">
-        <v>50.59007032135696</v>
+        <v>50.73686959720092</v>
       </c>
     </row>
     <row r="39">
@@ -592,7 +592,7 @@
         <v>31</v>
       </c>
       <c r="C40" t="n">
-        <v>1177.4215313358027</v>
+        <v>1180.8149251931632</v>
       </c>
     </row>
     <row r="41">
@@ -636,7 +636,7 @@
         <v>31</v>
       </c>
       <c r="C44" t="n">
-        <v>172135.1851118718</v>
+        <v>172623.83873822342</v>
       </c>
     </row>
     <row r="45">
@@ -658,7 +658,7 @@
         <v>31</v>
       </c>
       <c r="C46" t="n">
-        <v>63237.5879016962</v>
+        <v>63421.08699650115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on performance calculators.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
+++ b/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.2/Performance_0.2.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TAKE-OFF" r:id="rId3" sheetId="1"/>
+    <sheet name="NOISE TRAJECTORIES" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -23,109 +23,64 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Ground roll distance</t>
+    <t>SIDELINE ( 100% MAX-TO )</t>
+  </si>
+  <si>
+    <t>Ground distance</t>
   </si>
   <si>
     <t>m</t>
   </si>
   <si>
-    <t>Rotation distance</t>
-  </si>
-  <si>
-    <t>Airborne distance</t>
-  </si>
-  <si>
-    <t>AEO take-off distance</t>
-  </si>
-  <si>
-    <t>FAR-25 take-off field length</t>
-  </si>
-  <si>
-    <t>Balanced field length</t>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>Speed (TAS)</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>kts</t>
+  </si>
+  <si>
+    <t>Speed (CAS)</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>Thrust (x1 eng.)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>lbf</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ft</t>
-  </si>
-  <si>
-    <t>Stall speed take-off (VsTO)</t>
-  </si>
-  <si>
-    <t>m/s</t>
-  </si>
-  <si>
-    <t>Decision speed (V1)</t>
-  </si>
-  <si>
-    <t>Rotation speed (V_Rot)</t>
-  </si>
-  <si>
-    <t>Minimum control speed (VMC)</t>
-  </si>
-  <si>
-    <t>Lift-off speed (V_LO)</t>
-  </si>
-  <si>
-    <t>Take-off safety speed (V2)</t>
-  </si>
-  <si>
-    <t>kn</t>
-  </si>
-  <si>
-    <t>V1/VsTO</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>V_Rot/VsTO</t>
-  </si>
-  <si>
-    <t>VMC/VsTO</t>
-  </si>
-  <si>
-    <t>V_LO/VsTO</t>
-  </si>
-  <si>
-    <t>V2/VsTO</t>
-  </si>
-  <si>
-    <t>Take-off duration</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Take-off fuel used</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>Take-off NOx emissions</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Take-off CO emissions</t>
-  </si>
-  <si>
-    <t>Take-off HC emissions</t>
-  </si>
-  <si>
-    <t>Take-off Soot emissions</t>
-  </si>
-  <si>
-    <t>Take-off CO2 emissions</t>
-  </si>
-  <si>
-    <t>Take-off SOx emissions</t>
-  </si>
-  <si>
-    <t>Take-off H2O emissions</t>
+    <t>FLYOVER - CUTBACK ( 984.0ft, 47% MAX-TO )</t>
+  </si>
+  <si>
+    <t>APPROACH</t>
+  </si>
+  <si>
+    <t>Ground distance (from touch-down)</t>
   </si>
 </sst>
 </file>
@@ -212,33 +167,27 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>993.7163846639289</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" t="n">
-        <v>282.1452529462797</v>
+        <v>5085.190714335704</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="n">
-        <v>151.46515118137688</v>
+        <v>16683.696569342857</v>
       </c>
     </row>
     <row r="5">
@@ -246,419 +195,426 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>1427.3267887915854</v>
+        <v>650.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>1641.4258071103227</v>
+        <v>2132.54593175853</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" t="n">
-        <v>1853.2236402716744</v>
+        <v>76.74694127934654</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>149.18411911752025</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>3260.2243591336255</v>
+        <v>74.59706786181086</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>925.6734020547234</v>
+        <v>145.00509951539908</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" t="n">
-        <v>496.93291070005546</v>
+        <v>4.308393653936333</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>4682.830671888403</v>
+        <v>9.956084036909957</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>5385.255272671663</v>
+        <v>14.264477690846288</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C14" t="n">
-        <v>6080.130053384759</v>
+        <v>74480.20560952909</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="n">
+        <v>16743.816304927357</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="n">
-        <v>63.719070774443196</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="n">
-        <v>63.5085873574696</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>68.3549361418386</v>
+        <v>6500.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>59.750535586008674</v>
+        <v>21325.4593175853</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>74.326259768459</v>
+        <v>516.7796416654598</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>77.53034686818486</v>
+        <v>1695.471265306627</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="n">
+        <v>76.06241720050426</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C23" t="n">
-        <v>123.85996478833452</v>
+        <v>147.85351075691972</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>123.45081775750032</v>
+        <v>73.93171901127388</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>132.87136615044224</v>
+        <v>143.7117648167311</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C26" t="n">
-        <v>116.14574951923933</v>
+        <v>4.838393653936175</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C27" t="n">
-        <v>144.47869069462874</v>
+        <v>3.1349550318965917</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C28" t="n">
-        <v>150.70693775673084</v>
+        <v>7.973348685832766</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="n">
+        <v>35758.66289928127</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C30" t="n">
-        <v>0.9966966966966815</v>
+        <v>8038.867213046251</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1.0727547547547536</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.9377182507497229</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>1.1664680426926468</v>
+        <v>2265.805062777101</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C34" t="n">
-        <v>1.2167526287794068</v>
+        <v>7433.743644281826</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>120.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>34.11109999999999</v>
+        <v>393.70078740157476</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="n">
+        <v>65.31586091216067</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C38" t="n">
-        <v>50.73686959720092</v>
+        <v>126.9638765031201</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="n">
+        <v>66.82947489648434</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C40" t="n">
-        <v>1180.8149251931632</v>
+        <v>129.90610671022873</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0</v>
+        <v>0.6169530079361805</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0</v>
+        <v>-3.0368015768939802</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0</v>
+        <v>-2.4198485689578</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C44" t="n">
-        <v>172623.83873822342</v>
+        <v>246.60522063008096</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C45" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" t="n">
-        <v>63421.08699650115</v>
+        <v>55.43905901271942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>